<commit_message>
Fix checklist answer validation error
</commit_message>
<xml_diff>
--- a/bsb-be/src/main/resources/template/Inspection_Checklist_Template.xlsx
+++ b/bsb-be/src/main/resources/template/Inspection_Checklist_Template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99698120-CD5D-41D7-B653-7C1F1C3AB278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Item Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,13 +81,17 @@
   <si>
     <t>Follow-up 
 Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Section</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,78 +162,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -241,14 +178,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -316,6 +253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -351,6 +305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -526,23 +497,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="6.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
@@ -558,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
@@ -566,7 +537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
@@ -579,68 +550,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="12.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 G2:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 H2:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>action</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>action2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>